<commit_message>
Updated Command module and Discovery module
</commit_message>
<xml_diff>
--- a/Version.xlsx
+++ b/Version.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>1.1.1</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>Вынести зависимые функции наружу</t>
+  </si>
+  <si>
+    <t>1.2.44</t>
+  </si>
+  <si>
+    <t>Добавлена связь .well-known/core с коммандным модулем</t>
   </si>
 </sst>
 </file>
@@ -63,9 +69,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -367,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -380,24 +389,119 @@
     <col min="3" max="3" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>